<commit_message>
customers read  from excel done!!
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>EV type</t>
   </si>
@@ -30,15 +30,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>1: Nissan</t>
-  </si>
-  <si>
-    <t>2:Chev</t>
-  </si>
-  <si>
-    <t>3:Tesla</t>
   </si>
   <si>
     <t>2: CHAdeMO</t>
@@ -568,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -584,70 +575,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="E2" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -661,10 +652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F25" sqref="A20:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,13 +670,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -711,9 +702,7 @@
       <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>3</v>
-      </c>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -731,9 +720,7 @@
       <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>4</v>
-      </c>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -751,9 +738,7 @@
       <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -844,86 +829,6 @@
         <v>1</v>
       </c>
       <c r="F9" s="14"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5">
-        <v>1</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>2</v>
-      </c>
-      <c r="B22" s="5">
-        <v>4</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>3</v>
-      </c>
-      <c r="B23" s="5">
-        <v>2</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>4</v>
-      </c>
-      <c r="B24" s="5">
-        <v>2</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>5</v>
-      </c>
-      <c r="B25" s="5">
-        <v>3</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -932,10 +837,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G20:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,21 +851,21 @@
     <col min="4" max="4" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -968,13 +873,13 @@
         <v>0.375</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -982,13 +887,13 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D3" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -996,13 +901,13 @@
         <v>0.42986111111111108</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1010,13 +915,13 @@
         <v>0.375</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D5" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1024,13 +929,13 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1038,13 +943,13 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1052,16 +957,96 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
charger model done!! design plan added
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>EV type</t>
   </si>
@@ -652,10 +652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F25" sqref="A20:F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="A13:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +665,7 @@
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,6 +829,86 @@
         <v>1</v>
       </c>
       <c r="F9" s="14"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5">
+        <v>4</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -839,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="A12:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,6 +929,7 @@
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
charger mapping done!! excel file read done .
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>EV type</t>
   </si>
@@ -652,10 +652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="A13:F18"/>
+      <selection activeCell="A22" sqref="A22:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,85 +830,71 @@
       </c>
       <c r="F9" s="14"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="B22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>1</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B23" s="5">
         <v>1</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>2</v>
-      </c>
-      <c r="B15" s="5">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5">
         <v>4</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="15" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>4</v>
+      </c>
+      <c r="B26" s="5">
+        <v>2</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>5</v>
+      </c>
+      <c r="B27" s="5">
         <v>3</v>
       </c>
-      <c r="B16" s="5">
-        <v>2</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>4</v>
-      </c>
-      <c r="B17" s="5">
-        <v>2</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>5</v>
-      </c>
-      <c r="B18" s="5">
-        <v>3</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>